<commit_message>
Integration tests, some additional tweaks to formulae
</commit_message>
<xml_diff>
--- a/assets/abilities.xlsx
+++ b/assets/abilities.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ran Liu\PycharmProjects\keybind_generator\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F6AC76-6E15-4007-997D-D692F2B9C175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742DB253-CEE0-40BA-A39D-114AE750B3FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1755" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6683194F-2724-4542-99E4-27A65288EC1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{6683194F-2724-4542-99E4-27A65288EC1D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Magic DW Abilities" sheetId="1" r:id="rId1"/>
-    <sheet name="Magic Combinations" sheetId="2" r:id="rId2"/>
-    <sheet name="Melee DW Abilities" sheetId="3" r:id="rId3"/>
-    <sheet name="Melee Combinations" sheetId="4" r:id="rId4"/>
+    <sheet name="Key Layout" sheetId="6" r:id="rId1"/>
+    <sheet name="Magic DW Abilities" sheetId="1" r:id="rId2"/>
+    <sheet name="Magic Combinations" sheetId="2" r:id="rId3"/>
+    <sheet name="Magic Hand Binds" sheetId="5" r:id="rId4"/>
+    <sheet name="Scratch" sheetId="7" r:id="rId5"/>
+    <sheet name="Melee DW Abilities" sheetId="3" r:id="rId6"/>
+    <sheet name="Melee Combinations" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="214">
   <si>
     <t>Ability Name</t>
   </si>
@@ -390,9 +393,6 @@
     <t>Guthix Staff&gt;Special Attack&gt;Wand Switch&gt;Orb Switch</t>
   </si>
   <si>
-    <t>Desolation&gt;Seren Godbow&gt;Special Attack</t>
-  </si>
-  <si>
     <t>Ice Barrage&gt;Detonate&gt;Tsunami</t>
   </si>
   <si>
@@ -409,6 +409,276 @@
   </si>
   <si>
     <t>Deep Impact</t>
+  </si>
+  <si>
+    <t>Desolation&gt;Seren Godbow&gt;Ingenuity of the Humans&gt;Special Attack</t>
+  </si>
+  <si>
+    <t>Ice Barrage&gt;Detonate&gt;Dragon Breath</t>
+  </si>
+  <si>
+    <t>Blood Barrage&gt;Detonate&gt;Dragon Breath</t>
+  </si>
+  <si>
+    <t>Shield Switch&gt;Reflect</t>
+  </si>
+  <si>
+    <t>Defender Switch&gt;Reflect</t>
+  </si>
+  <si>
+    <t>Shield Switch&gt;Revenge</t>
+  </si>
+  <si>
+    <t>Defender Switch&gt;Revenge</t>
+  </si>
+  <si>
+    <t>Eat Food&gt;Saradomin Brew</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Keys</t>
+  </si>
+  <si>
+    <t>X-Offset</t>
+  </si>
+  <si>
+    <t>Y-Offset</t>
+  </si>
+  <si>
+    <t>Mouse Penalty</t>
+  </si>
+  <si>
+    <t>Modifier</t>
+  </si>
+  <si>
+    <t>Modifier Penalty</t>
+  </si>
+  <si>
+    <t>Bind</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>Shift+X</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Shift+Q</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Shift+1</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>Shift+2</t>
+  </si>
+  <si>
+    <t>Shift+3</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Shift+A</t>
+  </si>
+  <si>
+    <t>Shift+T</t>
+  </si>
+  <si>
+    <t>Shift+W</t>
+  </si>
+  <si>
+    <t>Shift+C</t>
+  </si>
+  <si>
+    <t>Shift+Z</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Shift+G</t>
+  </si>
+  <si>
+    <t>Shift+E</t>
+  </si>
+  <si>
+    <t>Shift+R</t>
+  </si>
+  <si>
+    <t>Shift+S</t>
+  </si>
+  <si>
+    <t>Shift+D</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>Alt+S</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>Alt+D</t>
+  </si>
+  <si>
+    <t>Shift+5</t>
+  </si>
+  <si>
+    <t>Shift+4</t>
+  </si>
+  <si>
+    <t>Alt+F</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>Alt+R</t>
+  </si>
+  <si>
+    <t>F7</t>
   </si>
 </sst>
 </file>
@@ -452,9 +722,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,11 +1044,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95196B6A-7609-4A1F-AA0D-73BEAAFB5614}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C60286-EF72-402C-B298-6B64A6B4C92A}">
   <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>74</v>
@@ -1052,7 +1371,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1063,7 +1382,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1605,7 +1924,7 @@
         <v>72</v>
       </c>
       <c r="B75">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C75" t="s">
         <v>75</v>
@@ -1639,17 +1958,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9A92560-C1D4-4ABC-88FC-7C94D8DEB9F1}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -1660,7 +1979,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>112</v>
@@ -1682,7 +2001,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1825,7 +2144,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1836,7 +2155,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1847,12 +2166,89 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1861,7 +2257,654 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31F1635-B516-4288-95EF-EB4DDEE5147E}">
+  <dimension ref="A1:B77"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>72</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBBAE2EF-520E-4902-95B2-89D4003D55B4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E688F0B-BBD4-41F6-8375-44791DA0D5AD}">
   <dimension ref="A1:D72"/>
   <sheetViews>
@@ -1882,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>74</v>
@@ -2464,7 +3507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBF0EC5-1789-4516-84AA-82940ADEB508}">
   <dimension ref="A1:D1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added evaluation of manual bindings
</commit_message>
<xml_diff>
--- a/assets/abilities.xlsx
+++ b/assets/abilities.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ran Liu\PycharmProjects\keybind_generator\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742DB253-CEE0-40BA-A39D-114AE750B3FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E419C0A-A348-478D-BD65-D1785A8DEAD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{6683194F-2724-4542-99E4-27A65288EC1D}"/>
+    <workbookView xWindow="28680" yWindow="-1755" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6683194F-2724-4542-99E4-27A65288EC1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Key Layout" sheetId="6" r:id="rId1"/>
     <sheet name="Magic DW Abilities" sheetId="1" r:id="rId2"/>
     <sheet name="Magic Combinations" sheetId="2" r:id="rId3"/>
     <sheet name="Magic Hand Binds" sheetId="5" r:id="rId4"/>
-    <sheet name="Scratch" sheetId="7" r:id="rId5"/>
-    <sheet name="Melee DW Abilities" sheetId="3" r:id="rId6"/>
-    <sheet name="Melee Combinations" sheetId="4" r:id="rId7"/>
+    <sheet name="Melee DW Abilities" sheetId="3" r:id="rId5"/>
+    <sheet name="Melee Combinations" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="226">
   <si>
     <t>Ability Name</t>
   </si>
@@ -465,9 +464,6 @@
     <t>Shift+X</t>
   </si>
   <si>
-    <t>;</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -480,9 +476,6 @@
     <t>Shift+Q</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -492,12 +485,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>\</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -531,30 +518,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
@@ -570,12 +533,6 @@
     <t>Shift+3</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -618,15 +575,6 @@
     <t>G</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -636,9 +584,6 @@
     <t>Alt+S</t>
   </si>
   <si>
-    <t>Delete</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
@@ -651,15 +596,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>Insert</t>
-  </si>
-  <si>
-    <t>]</t>
-  </si>
-  <si>
-    <t>[</t>
-  </si>
-  <si>
     <t>Alt+D</t>
   </si>
   <si>
@@ -672,13 +608,112 @@
     <t>Alt+F</t>
   </si>
   <si>
-    <t>F8</t>
-  </si>
-  <si>
     <t>Alt+R</t>
   </si>
   <si>
-    <t>F7</t>
+    <t>Keyboard</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>Q,W,E,R,T,Y</t>
+  </si>
+  <si>
+    <t>Priorities</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Group Penalty</t>
+  </si>
+  <si>
+    <t>A,S,D,F,G,H</t>
+  </si>
+  <si>
+    <t>Q,W,E,R,T</t>
+  </si>
+  <si>
+    <t>A,S,D,F,G</t>
+  </si>
+  <si>
+    <t>Alt</t>
+  </si>
+  <si>
+    <t>Z,X,C,V,B,N</t>
+  </si>
+  <si>
+    <t>Z,X,C,V,B</t>
+  </si>
+  <si>
+    <t>Mouse1</t>
+  </si>
+  <si>
+    <t>Mouse2</t>
+  </si>
+  <si>
+    <t>Mouse3</t>
+  </si>
+  <si>
+    <t>Mouse4</t>
+  </si>
+  <si>
+    <t>Mouse5</t>
+  </si>
+  <si>
+    <t>Mouse6</t>
+  </si>
+  <si>
+    <t>Mouse7</t>
+  </si>
+  <si>
+    <t>Mouse8</t>
+  </si>
+  <si>
+    <t>Shift+Mouse1</t>
+  </si>
+  <si>
+    <t>Shift+Mouse2</t>
+  </si>
+  <si>
+    <t>Shift+Mouse4</t>
+  </si>
+  <si>
+    <t>Mouse9</t>
+  </si>
+  <si>
+    <t>Mouse10</t>
+  </si>
+  <si>
+    <t>Mouse11</t>
+  </si>
+  <si>
+    <t>Mouse12</t>
+  </si>
+  <si>
+    <t>F1,F2,F3,F4,F5,F6</t>
+  </si>
+  <si>
+    <t>Alt+A</t>
+  </si>
+  <si>
+    <t>Shift+Mouse3</t>
+  </si>
+  <si>
+    <t>Shift+Mouse6</t>
+  </si>
+  <si>
+    <t>Shift+Mouse5</t>
+  </si>
+  <si>
+    <t>Shift+Mouse9</t>
+  </si>
+  <si>
+    <t>Shift+Mouse7</t>
   </si>
 </sst>
 </file>
@@ -722,13 +757,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1045,7 +1093,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95196B6A-7609-4A1F-AA0D-73BEAAFB5614}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1053,31 +1101,256 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="4"/>
+    <col min="8" max="8" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="4"/>
+    <col min="10" max="10" width="16.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="J4" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="J6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J7" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="G8" s="4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="J9" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="G10" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J10" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="J12" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J13" s="4">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2261,14 +2534,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31F1635-B516-4288-95EF-EB4DDEE5147E}">
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="1" max="1" width="23.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2280,631 +2553,620 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="8" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="3" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="3" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="3" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="3" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="3" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="3" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="3" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>122</v>
-      </c>
-      <c r="B26" s="3" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="3" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="3" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="3" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="3" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="3" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="3" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="3" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="3" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="3" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36" s="3" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="3" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="3" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="3" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="3" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="3" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="3" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="3" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="3" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="3" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="3" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="8" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="3" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" s="3" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="8" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" s="3" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="8" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" s="3" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="3" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" s="3" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>53</v>
-      </c>
-      <c r="B54" s="3" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" s="8" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>54</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>57</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>58</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>67</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>68</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>69</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>80</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>72</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>73</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>213</v>
+      <c r="B77" s="8" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBBAE2EF-520E-4902-95B2-89D4003D55B4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E688F0B-BBD4-41F6-8375-44791DA0D5AD}">
   <dimension ref="A1:D72"/>
   <sheetViews>
@@ -3507,7 +3769,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBF0EC5-1789-4516-84AA-82940ADEB508}">
   <dimension ref="A1:D1"/>
   <sheetViews>

</xml_diff>